<commit_message>
Aggiornamento calcolo dei garanti
Molti file sono segnati come modificati per modifica dei permessi
</commit_message>
<xml_diff>
--- a/src/dataset/allegato-d-sanitized.xlsx
+++ b/src/dataset/allegato-d-sanitized.xlsx
@@ -594,7 +594,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>L/ShT4</t>
+          <t>L/SNT4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>L-Sc. Mat.</t>
+          <t>L-Sc.Mat.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>L4</t>
+          <t>L-4</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>LP-01</t>
+          <t>L-P01</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LP-02</t>
+          <t>L-P02</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>LP-03</t>
+          <t>L-P03</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2582,7 +2582,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>LM-I7</t>
+          <t>LM-17</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2605,13 +2605,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2634,13 +2642,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2663,13 +2679,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2692,13 +2716,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2721,13 +2753,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2750,13 +2790,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2779,13 +2827,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr"/>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2808,13 +2864,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2837,13 +2901,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2866,13 +2938,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2895,13 +2975,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2924,13 +3012,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2953,13 +3049,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2982,13 +3086,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3011,13 +3123,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3040,13 +3160,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3069,13 +3197,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr"/>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3098,13 +3234,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3127,13 +3271,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3156,13 +3308,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3185,13 +3345,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3214,13 +3382,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr"/>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3243,13 +3419,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3272,13 +3456,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="inlineStr"/>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3301,13 +3493,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3330,13 +3530,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3359,13 +3567,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3388,13 +3604,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3417,13 +3641,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr"/>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3446,13 +3678,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3475,13 +3715,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3504,13 +3752,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3533,13 +3789,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3562,13 +3826,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3591,13 +3863,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -3620,13 +3900,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3649,13 +3937,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3678,13 +3974,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3707,13 +4011,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3736,13 +4048,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3765,13 +4085,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3794,13 +4122,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3823,13 +4159,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3852,13 +4196,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr"/>
-      <c r="G102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3881,13 +4233,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3910,13 +4270,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -3939,13 +4307,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3968,13 +4344,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3997,13 +4381,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -4026,13 +4418,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -4055,13 +4455,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr"/>
-      <c r="G109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -4084,13 +4492,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr"/>
-      <c r="G110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -4113,13 +4529,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -4142,13 +4566,21 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr"/>
-      <c r="G112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -4171,8 +4603,16 @@
           <t>LM</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5778,7 +6218,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>LM—42</t>
+          <t>LM-42</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -5805,7 +6245,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -5828,13 +6268,21 @@
           <t>LMCU</t>
         </is>
       </c>
-      <c r="F158" t="inlineStr"/>
-      <c r="G158" t="inlineStr"/>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -5857,13 +6305,21 @@
           <t>LMCU</t>
         </is>
       </c>
-      <c r="F159" t="inlineStr"/>
-      <c r="G159" t="inlineStr"/>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>scientifico tecnologica</t>
+          <t>scientifico tecnologico</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -5886,8 +6342,16 @@
           <t>LMCU</t>
         </is>
       </c>
-      <c r="F160" t="inlineStr"/>
-      <c r="G160" t="inlineStr"/>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">

</xml_diff>